<commit_message>
statistics for new release
</commit_message>
<xml_diff>
--- a/intenz-database/src/site/resources/statistics/intenzStats-2012.xlsx
+++ b/intenz-database/src/site/resources/statistics/intenzStats-2012.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="364" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="363" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" state="visible" r:id="rId2"/>
@@ -127,10 +127,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="YYYY\-MM\-DD" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="166"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -296,11 +295,10 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
@@ -380,7 +378,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -412,7 +410,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$8</c:f>
+              <c:f>Table!$A$8:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -455,7 +453,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -503,7 +501,7 @@
                   <c:v>4866</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>4929</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -532,7 +530,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$9</c:f>
+              <c:f>Table!$A$9:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -575,7 +573,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -623,7 +621,7 @@
                   <c:v>820</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -652,7 +650,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$10</c:f>
+              <c:f>Table!$A$10:$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -695,7 +693,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -743,7 +741,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -772,7 +770,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$11</c:f>
+              <c:f>Table!$A$11:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -815,7 +813,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -863,7 +861,7 @@
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -892,7 +890,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$12</c:f>
+              <c:f>Table!$A$12:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -935,7 +933,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1012,7 +1010,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$13</c:f>
+              <c:f>Table!$A$13:$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1055,7 +1053,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1132,7 +1130,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$14</c:f>
+              <c:f>Table!$A$14:$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1175,7 +1173,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1223,7 +1221,7 @@
                   <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -1252,7 +1250,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$15</c:f>
+              <c:f>Table!$A$15:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1295,7 +1293,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1369,11 +1367,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="38510873"/>
-        <c:axId val="69437030"/>
+        <c:axId val="54917625"/>
+        <c:axId val="48207922"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38510873"/>
+        <c:axId val="54917625"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1399,7 +1397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="69437030"/>
+        <c:crossAx val="48207922"/>
         <c:crossesAt val="3000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1413,7 +1411,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69437030"/>
+        <c:axId val="48207922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="3000"/>
@@ -1454,7 +1452,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38510873"/>
+        <c:crossAx val="54917625"/>
         <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
@@ -1486,7 +1484,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1518,7 +1516,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$43</c:f>
+              <c:f>Table!$A$43:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1561,7 +1559,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1609,7 +1607,7 @@
                   <c:v>5686</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>5754</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1638,7 +1636,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$44</c:f>
+              <c:f>Table!$A$44:$A$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1681,7 +1679,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1729,7 +1727,7 @@
                   <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>181</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1758,7 +1756,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$45</c:f>
+              <c:f>Table!$A$45:$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1801,7 +1799,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -1846,7 +1844,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>99</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1875,11 +1873,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="78130265"/>
-        <c:axId val="43159937"/>
+        <c:axId val="47379245"/>
+        <c:axId val="38907458"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78130265"/>
+        <c:axId val="47379245"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1905,7 +1903,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="43159937"/>
+        <c:crossAx val="38907458"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1919,7 +1917,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43159937"/>
+        <c:axId val="38907458"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4600"/>
@@ -1960,7 +1958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78130265"/>
+        <c:crossAx val="47379245"/>
         <c:crosses val="min"/>
         <c:majorUnit val="100"/>
         <c:minorUnit val="50"/>
@@ -1994,7 +1992,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2026,7 +2024,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$27</c:f>
+              <c:f>Table!$A$27:$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2069,7 +2067,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2117,7 +2115,7 @@
                   <c:v>3388</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>3383</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2146,7 +2144,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$28</c:f>
+              <c:f>Table!$A$28:$A$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2189,7 +2187,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2237,7 +2235,7 @@
                   <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2266,7 +2264,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$29</c:f>
+              <c:f>Table!$A$29:$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2309,7 +2307,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2357,7 +2355,7 @@
                   <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2386,7 +2384,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$30</c:f>
+              <c:f>Table!$A$30:$A$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2429,7 +2427,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2477,7 +2475,7 @@
                   <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2506,7 +2504,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$31</c:f>
+              <c:f>Table!$A$31:$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2549,7 +2547,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2597,7 +2595,7 @@
                   <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2626,7 +2624,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$32</c:f>
+              <c:f>Table!$A$32:$A$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2669,7 +2667,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2717,7 +2715,7 @@
                   <c:v>740</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -2743,11 +2741,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="27680918"/>
-        <c:axId val="97025473"/>
+        <c:axId val="787028"/>
+        <c:axId val="44053136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="27680918"/>
+        <c:axId val="787028"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2778,7 +2776,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="97025473"/>
+        <c:crossAx val="44053136"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -2792,7 +2790,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97025473"/>
+        <c:axId val="44053136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2832,7 +2830,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="27680918"/>
+        <c:crossAx val="787028"/>
         <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
@@ -2864,7 +2862,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2896,7 +2894,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$25</c:f>
+              <c:f>Table!$A$25:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2939,7 +2937,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -2987,7 +2985,7 @@
                   <c:v>207555</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>207470</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3016,7 +3014,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$23</c:f>
+              <c:f>Table!$A$23:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3059,7 +3057,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3107,7 +3105,7 @@
                   <c:v>3990</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>3985</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3136,7 +3134,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$24</c:f>
+              <c:f>Table!$A$24:$A$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3179,7 +3177,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3227,7 +3225,7 @@
                   <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3256,7 +3254,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$22</c:f>
+              <c:f>Table!$A$22:$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3299,7 +3297,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3347,7 +3345,7 @@
                   <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3373,11 +3371,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="63525927"/>
-        <c:axId val="94165507"/>
+        <c:axId val="91872716"/>
+        <c:axId val="56974197"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63525927"/>
+        <c:axId val="91872716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3385,7 +3383,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="94165507"/>
+        <c:crossAx val="56974197"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -3399,7 +3397,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94165507"/>
+        <c:axId val="56974197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -3440,7 +3438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63525927"/>
+        <c:crossAx val="91872716"/>
         <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
@@ -3472,7 +3470,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3504,7 +3502,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$20</c:f>
+              <c:f>Table!$A$20:$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3547,7 +3545,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3595,7 +3593,7 @@
                   <c:v>218027</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>217964</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3624,7 +3622,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$18</c:f>
+              <c:f>Table!$A$18:$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3667,7 +3665,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3715,7 +3713,7 @@
                   <c:v>4017</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>4012</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3744,7 +3742,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$19</c:f>
+              <c:f>Table!$A$19:$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3787,7 +3785,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3835,7 +3833,7 @@
                   <c:v>1442</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>1442</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3864,7 +3862,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Table!$A$17</c:f>
+              <c:f>Table!$A$17:$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3907,7 +3905,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -3955,7 +3953,7 @@
                   <c:v>1548</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>NaN</c:v>
+                  <c:v>1548</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>NaN</c:v>
@@ -3981,11 +3979,11 @@
         </c:ser>
         <c:overlap val="100"/>
         <c:gapWidth val="100"/>
-        <c:axId val="108801"/>
-        <c:axId val="46787517"/>
+        <c:axId val="39992197"/>
+        <c:axId val="92735023"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="108801"/>
+        <c:axId val="39992197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3993,7 +3991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="46787517"/>
+        <c:crossAx val="92735023"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -4007,7 +4005,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46787517"/>
+        <c:axId val="92735023"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="160000"/>
@@ -4048,7 +4046,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108801"/>
+        <c:crossAx val="39992197"/>
         <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
@@ -4080,7 +4078,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4132,7 +4130,7 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v/>
@@ -4183,7 +4181,7 @@
                   <c:v>19030</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>NaN</c:v>
+                  <c:v>19217</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>NaN</c:v>
@@ -4208,11 +4206,11 @@
           </c:val>
         </c:ser>
         <c:marker val="0"/>
-        <c:axId val="64740573"/>
-        <c:axId val="86254139"/>
+        <c:axId val="8985573"/>
+        <c:axId val="93159410"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64740573"/>
+        <c:axId val="8985573"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4243,7 +4241,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="86254139"/>
+        <c:crossAx val="93159410"/>
         <c:crossesAt val="17000"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -4257,7 +4255,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86254139"/>
+        <c:axId val="93159410"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4298,7 +4296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64740573"/>
+        <c:crossAx val="8985573"/>
         <c:crosses val="min"/>
         <c:spPr>
           <a:ln>
@@ -4331,13 +4329,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>165600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>1080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>83880</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>1800</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4345,8 +4343,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="165600" y="154080"/>
-        <a:ext cx="11590200" cy="3706560"/>
+        <a:off x="165600" y="160200"/>
+        <a:ext cx="11590200" cy="3836880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4361,7 +4359,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>152280</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -4375,8 +4373,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="152280" y="3946320"/>
-        <a:ext cx="11638800" cy="3603600"/>
+        <a:off x="152280" y="4081680"/>
+        <a:ext cx="11638800" cy="3740760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4411,7 +4409,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="56160"/>
-        <a:ext cx="11962440" cy="3672360"/>
+        <a:ext cx="11962440" cy="3803760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4435,9 +4433,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>495720</xdr:colOff>
+      <xdr:colOff>491760</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4446,7 +4444,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="292680" y="19440"/>
-        <a:ext cx="11249280" cy="3535200"/>
+        <a:ext cx="11245320" cy="3661200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4461,13 +4459,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>318600</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>525960</xdr:colOff>
+      <xdr:colOff>522000</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>88920</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4475,8 +4473,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="318600" y="3711600"/>
-        <a:ext cx="11253600" cy="3630240"/>
+        <a:off x="318600" y="3843360"/>
+        <a:ext cx="11249640" cy="3769200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4502,7 +4500,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>75600</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4511,7 +4509,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="59400" y="51840"/>
-        <a:ext cx="10968480" cy="3723120"/>
+        <a:ext cx="10968480" cy="3861360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4532,7 +4530,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H1" activeCellId="0" pane="topLeft" sqref="H1"/>
+      <selection activeCell="I1" activeCellId="0" pane="topLeft" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -4540,7 +4538,7 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.4862745098039"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1" s="1">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="1" s="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4562,8 +4560,11 @@
       <c r="G1" s="1" t="n">
         <v>80</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="H1" s="1" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -4585,11 +4586,17 @@
       <c r="G2" s="2" t="n">
         <v>41159</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="H2" s="2" t="n">
+        <v>41190</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -4611,8 +4618,11 @@
       <c r="G3" s="0" t="n">
         <v>6</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="H3" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -4634,8 +4644,11 @@
       <c r="G4" s="0" t="n">
         <v>67</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="H4" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -4657,13 +4670,15 @@
       <c r="G5" s="0" t="n">
         <v>285</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="H5" s="3" t="n">
+        <v>285</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="n">
+      <c r="B6" s="4" t="n">
         <v>18771</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -4681,20 +4696,22 @@
       <c r="G6" s="0" t="n">
         <v>19030</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="H6" s="3" t="n">
+        <v>19217</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="7">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="4"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="n">
+      <c r="B8" s="4" t="n">
         <v>4731</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -4712,13 +4729,15 @@
       <c r="G8" s="0" t="n">
         <v>4866</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="5" t="s">
+      <c r="H8" s="3" t="n">
+        <v>4929</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="9">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="n">
+      <c r="B9" s="4" t="n">
         <v>805</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -4736,12 +4755,15 @@
       <c r="G9" s="0" t="n">
         <v>820</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="5" t="s">
+      <c r="H9" s="0" t="n">
+        <v>825</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="10">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="4" t="n">
         <v>71</v>
       </c>
       <c r="C10" s="0" t="n">
@@ -4759,12 +4781,15 @@
       <c r="G10" s="0" t="n">
         <v>80</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="5" t="s">
+      <c r="H10" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="11">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="n">
+      <c r="B11" s="4" t="n">
         <v>79</v>
       </c>
       <c r="C11" s="0" t="n">
@@ -4782,12 +4807,15 @@
       <c r="G11" s="0" t="n">
         <v>101</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="5" t="s">
+      <c r="H11" s="0" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="12">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -4803,35 +4831,38 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="13">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="5"/>
+      <c r="B13" s="4"/>
       <c r="E13" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="14">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="0" t="n">
         <v>99</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="5" t="s">
+      <c r="H14" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="15">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="17">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -4852,9 +4883,12 @@
       <c r="G17" s="0" t="n">
         <v>1548</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="A18" s="5" t="s">
+      <c r="H17" s="0" t="n">
+        <v>1548</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="18">
+      <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="0" t="n">
@@ -4875,9 +4909,12 @@
       <c r="G18" s="0" t="n">
         <v>4017</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="A19" s="5" t="s">
+      <c r="H18" s="0" t="n">
+        <v>4012</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="19">
+      <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="0" t="n">
@@ -4898,9 +4935,12 @@
       <c r="G19" s="0" t="n">
         <v>1442</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="20">
-      <c r="A20" s="5" t="s">
+      <c r="H19" s="0" t="n">
+        <v>1442</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="0" t="n">
@@ -4921,14 +4961,17 @@
       <c r="G20" s="0" t="n">
         <v>218027</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="21">
+      <c r="H20" s="0" t="n">
+        <v>217964</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
-      <c r="A22" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="22">
+      <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B22" s="0" t="n">
@@ -4949,9 +4992,12 @@
       <c r="G22" s="0" t="n">
         <v>509</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="23">
-      <c r="A23" s="5" t="s">
+      <c r="H22" s="0" t="n">
+        <v>509</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="23">
+      <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="0" t="n">
@@ -4972,9 +5018,12 @@
       <c r="G23" s="0" t="n">
         <v>3990</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="24">
-      <c r="A24" s="5" t="s">
+      <c r="H23" s="0" t="n">
+        <v>3985</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="24">
+      <c r="A24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B24" s="0" t="n">
@@ -4995,9 +5044,12 @@
       <c r="G24" s="0" t="n">
         <v>466</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="25">
-      <c r="A25" s="5" t="s">
+      <c r="H24" s="0" t="n">
+        <v>466</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="25">
+      <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="0" t="n">
@@ -5018,14 +5070,17 @@
       <c r="G25" s="0" t="n">
         <v>207555</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="26">
+      <c r="H25" s="0" t="n">
+        <v>207470</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="27">
-      <c r="A27" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="27">
+      <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="0" t="n">
@@ -5046,9 +5101,12 @@
       <c r="G27" s="0" t="n">
         <v>3388</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="28">
-      <c r="A28" s="5" t="s">
+      <c r="H27" s="0" t="n">
+        <v>3383</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="28">
+      <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="0" t="n">
@@ -5069,9 +5127,12 @@
       <c r="G28" s="0" t="n">
         <v>68</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="29">
-      <c r="A29" s="5" t="s">
+      <c r="H28" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="29">
+      <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="0" t="n">
@@ -5092,9 +5153,12 @@
       <c r="G29" s="0" t="n">
         <v>344</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="30">
-      <c r="A30" s="5" t="s">
+      <c r="H29" s="0" t="n">
+        <v>344</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="30">
+      <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="0" t="n">
@@ -5115,9 +5179,12 @@
       <c r="G30" s="0" t="n">
         <v>352</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="31">
-      <c r="A31" s="5" t="s">
+      <c r="H30" s="0" t="n">
+        <v>352</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="31">
+      <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="0" t="n">
@@ -5138,9 +5205,12 @@
       <c r="G31" s="0" t="n">
         <v>218</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="32">
-      <c r="A32" s="5" t="s">
+      <c r="H31" s="0" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="32">
+      <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="0" t="n">
@@ -5161,14 +5231,17 @@
       <c r="G32" s="0" t="n">
         <v>740</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="33">
+      <c r="H32" s="0" t="n">
+        <v>724</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="33">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="34">
-      <c r="A34" s="5" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="34">
+      <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -5189,9 +5262,12 @@
       <c r="G34" s="0" t="n">
         <v>3219</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="35">
-      <c r="A35" s="5" t="s">
+      <c r="H34" s="0" t="n">
+        <v>3214</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="35">
+      <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -5212,9 +5288,12 @@
       <c r="G35" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="36">
-      <c r="A36" s="5" t="s">
+      <c r="H35" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="36">
+      <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -5235,12 +5314,15 @@
       <c r="G36" s="0" t="n">
         <v>337</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="37">
-      <c r="A37" s="5" t="s">
+      <c r="H36" s="0" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="37">
+      <c r="A37" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="5" t="n">
+      <c r="B37" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="0" t="n">
@@ -5258,12 +5340,15 @@
       <c r="G37" s="0" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="38">
-      <c r="A38" s="5" t="s">
+      <c r="H37" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="38">
+      <c r="A38" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="5" t="n">
+      <c r="B38" s="4" t="n">
         <v>79</v>
       </c>
       <c r="C38" s="0" t="n">
@@ -5281,12 +5366,15 @@
       <c r="G38" s="0" t="n">
         <v>78</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="39">
-      <c r="A39" s="5" t="s">
+      <c r="H38" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="39">
+      <c r="A39" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="5" t="n">
+      <c r="B39" s="4" t="n">
         <v>697</v>
       </c>
       <c r="C39" s="0" t="n">
@@ -5304,188 +5392,191 @@
       <c r="G39" s="0" t="n">
         <v>679</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+      <c r="H39" s="0" t="n">
+        <v>667</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="40">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="42">
       <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B42" s="1"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="43" s="5">
-      <c r="A43" s="5" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="43" s="4">
+      <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="5" t="n">
+      <c r="B43" s="4" t="n">
         <f aca="false">SUM(B8:B9)</f>
         <v>5536</v>
       </c>
-      <c r="C43" s="5" t="n">
+      <c r="C43" s="4" t="n">
         <f aca="false">SUM(C8:C9)</f>
         <v>5536</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="D43" s="4" t="n">
         <f aca="false">SUM(D8:D9)</f>
         <v>5580</v>
       </c>
-      <c r="E43" s="5" t="n">
+      <c r="E43" s="4" t="n">
         <f aca="false">SUM(E8:E9)</f>
         <v>5654</v>
       </c>
-      <c r="F43" s="5" t="n">
+      <c r="F43" s="4" t="n">
         <f aca="false">SUM(F8:F9)</f>
         <v>5683</v>
       </c>
-      <c r="G43" s="5" t="n">
+      <c r="G43" s="4" t="n">
         <f aca="false">SUM(G8:G9)</f>
         <v>5686</v>
       </c>
-      <c r="H43" s="5" t="n">
+      <c r="H43" s="4" t="n">
         <f aca="false">SUM(H8:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="I43" s="5" t="n">
+        <v>5754</v>
+      </c>
+      <c r="I43" s="4" t="n">
         <f aca="false">SUM(I8:I9)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="5" t="n">
+      <c r="J43" s="4" t="n">
         <f aca="false">SUM(J8:J9)</f>
         <v>0</v>
       </c>
-      <c r="K43" s="5" t="n">
+      <c r="K43" s="4" t="n">
         <f aca="false">SUM(K8:K9)</f>
         <v>0</v>
       </c>
-      <c r="L43" s="5" t="n">
+      <c r="L43" s="4" t="n">
         <f aca="false">SUM(L8:L9)</f>
         <v>0</v>
       </c>
-      <c r="M43" s="5" t="n">
+      <c r="M43" s="4" t="n">
         <f aca="false">SUM(M8:M9)</f>
         <v>0</v>
       </c>
-      <c r="N43" s="5" t="n">
+      <c r="N43" s="4" t="n">
         <f aca="false">SUM(N8:N9)</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="44" s="5">
-      <c r="A44" s="5" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="44" s="4">
+      <c r="A44" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="5" t="n">
+      <c r="B44" s="4" t="n">
         <f aca="false">SUM(B10:B11)</f>
         <v>150</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="4" t="n">
         <f aca="false">SUM(C10:C11)</f>
         <v>161</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="4" t="n">
         <f aca="false">SUM(D10:D11)</f>
         <v>164</v>
       </c>
-      <c r="E44" s="5" t="n">
+      <c r="E44" s="4" t="n">
         <f aca="false">SUM(E10:E11)</f>
         <v>171</v>
       </c>
-      <c r="F44" s="5" t="n">
+      <c r="F44" s="4" t="n">
         <f aca="false">SUM(F10:F11)</f>
         <v>171</v>
       </c>
-      <c r="G44" s="5" t="n">
+      <c r="G44" s="4" t="n">
         <f aca="false">SUM(G10:G11)</f>
         <v>181</v>
       </c>
-      <c r="H44" s="5" t="n">
+      <c r="H44" s="4" t="n">
         <f aca="false">SUM(H10:H11)</f>
-        <v>0</v>
-      </c>
-      <c r="I44" s="5" t="n">
+        <v>181</v>
+      </c>
+      <c r="I44" s="4" t="n">
         <f aca="false">SUM(I10:I11)</f>
         <v>0</v>
       </c>
-      <c r="J44" s="5" t="n">
+      <c r="J44" s="4" t="n">
         <f aca="false">SUM(J10:J11)</f>
         <v>0</v>
       </c>
-      <c r="K44" s="5" t="n">
+      <c r="K44" s="4" t="n">
         <f aca="false">SUM(K10:K11)</f>
         <v>0</v>
       </c>
-      <c r="L44" s="5" t="n">
+      <c r="L44" s="4" t="n">
         <f aca="false">SUM(L10:L11)</f>
         <v>0</v>
       </c>
-      <c r="M44" s="5" t="n">
+      <c r="M44" s="4" t="n">
         <f aca="false">SUM(M10:M11)</f>
         <v>0</v>
       </c>
-      <c r="N44" s="5" t="n">
+      <c r="N44" s="4" t="n">
         <f aca="false">SUM(N10:N11)</f>
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="45" s="5">
-      <c r="A45" s="5" t="s">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="45" s="4">
+      <c r="A45" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="5" t="n">
+      <c r="B45" s="4" t="n">
         <f aca="false">B12</f>
         <v>1</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="4" t="n">
         <f aca="false">C12</f>
         <v>61</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="D45" s="4" t="n">
         <f aca="false">D12</f>
         <v>60</v>
       </c>
-      <c r="E45" s="5" t="n">
+      <c r="E45" s="4" t="n">
         <f aca="false">E12</f>
         <v>30</v>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="4" t="n">
         <f aca="false">F12</f>
         <v>2</v>
       </c>
-      <c r="G45" s="5" t="n">
-        <f aca="false">G14</f>
-        <v>99</v>
-      </c>
-      <c r="H45" s="5" t="n">
+      <c r="G45" s="4" t="n">
+        <f aca="false">G12</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="4" t="n">
         <f aca="false">H12</f>
         <v>0</v>
       </c>
-      <c r="I45" s="5" t="n">
+      <c r="I45" s="4" t="n">
         <f aca="false">I12</f>
         <v>0</v>
       </c>
-      <c r="J45" s="5" t="n">
+      <c r="J45" s="4" t="n">
         <f aca="false">J12</f>
         <v>0</v>
       </c>
-      <c r="K45" s="5" t="n">
+      <c r="K45" s="4" t="n">
         <f aca="false">K12</f>
         <v>0</v>
       </c>
-      <c r="L45" s="5" t="n">
+      <c r="L45" s="4" t="n">
         <f aca="false">L12</f>
         <v>0</v>
       </c>
-      <c r="M45" s="5" t="n">
+      <c r="M45" s="4" t="n">
         <f aca="false">M12</f>
         <v>0</v>
       </c>
-      <c r="N45" s="5" t="n">
+      <c r="N45" s="4" t="n">
         <f aca="false">N12</f>
         <v>0</v>
       </c>
@@ -5519,196 +5610,196 @@
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.41176470588235"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="1">
       <c r="C1" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="2">
       <c r="C2" s="1"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="H2" s="5"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="3">
       <c r="C3" s="1"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="G3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="4">
       <c r="C4" s="1"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="D8" s="4"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="D10" s="4"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="4"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="D11" s="4"/>
-      <c r="E11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="4"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="G4" s="5"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="5">
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="6">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="7">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="8">
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="9">
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="10">
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="11">
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="12">
       <c r="C12" s="1"/>
-      <c r="D12" s="4"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="D12" s="3"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="13">
       <c r="C13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="G13" s="5"/>
+      <c r="H13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="14">
       <c r="C14" s="1"/>
-      <c r="J14" s="4"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="J14" s="3"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="15">
       <c r="C15" s="1"/>
-      <c r="J15" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="J15" s="3"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="16">
       <c r="C16" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="17">
       <c r="C17" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="18">
       <c r="C18" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="19">
       <c r="C19" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="20">
       <c r="C20" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="21">
       <c r="C21" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.45" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
       <c r="C22" s="1"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4" t="s">
+      <c r="M22" s="5"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5740,7 +5831,7 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.28627450980392"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
     </row>
   </sheetData>
@@ -5770,12 +5861,12 @@
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.15686274509804"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.55" outlineLevel="0" r="1">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>